<commit_message>
Pedra da Cidade adicionada
</commit_message>
<xml_diff>
--- a/Traduzido/PTBR/Lang/PTBR/Dialog/Drama/_tutorial.xlsx
+++ b/Traduzido/PTBR/Lang/PTBR/Dialog/Drama/_tutorial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Dialog\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Dialog\Drama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690616B7-528B-4A71-9697-392805B379EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45460C25-9484-4E7E-82F2-FAE9DCCF4A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7875" yWindow="3060" windowWidth="17790" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2447,102 +2447,6 @@
     <t xml:space="preserve">Eu sei que é difícil, mas aguente firme... </t>
   </si>
   <si>
-    <t xml:space="preserve">Sono e Descanso  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mapa Global  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fama  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminoso  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fim da Infância  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Água Perigosa  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasto e Gado  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dureza dos Materiais  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fé e Orações  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doença do Éter  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caixa de Entregas  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problema com o Lixo  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">O Início da Aventura  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como Usar as Ferramentas  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algo Muito Importante  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Importância dos Equipamentos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Situação dos Alimentos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Materiais Processados  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Características dos Itens  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crescimento e Talentos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carma  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enfraquecimento e Recuperação  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deterioração dos Equipamentos por Ácido  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morte e Consequências  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ressurreição de Companheiros e Moradores  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ponto de Parada do Mercador Viajante  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cidade  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grau de Influência  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedra do Pacto  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trabalhos e Hobbies dos Moradores  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estações do Ano  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nerun Demo  </t>
-  </si>
-  <si>
     <t>Alerta de Inverno</t>
   </si>
   <si>
@@ -2944,6 +2848,102 @@
   </si>
   <si>
     <t>... E então?</t>
+  </si>
+  <si>
+    <t>O Início da Aventura</t>
+  </si>
+  <si>
+    <t>Como Usar as Ferramentas</t>
+  </si>
+  <si>
+    <t>Algo Muito Importante</t>
+  </si>
+  <si>
+    <t>A Importância dos Equipamentos</t>
+  </si>
+  <si>
+    <t>Situação dos Alimentos</t>
+  </si>
+  <si>
+    <t>Materiais Processados</t>
+  </si>
+  <si>
+    <t>Dureza dos Materiais</t>
+  </si>
+  <si>
+    <t>Sono e Descanso</t>
+  </si>
+  <si>
+    <t>Características dos Itens</t>
+  </si>
+  <si>
+    <t>Mapa Global</t>
+  </si>
+  <si>
+    <t>Crescimento e Talentos</t>
+  </si>
+  <si>
+    <t>Fama</t>
+  </si>
+  <si>
+    <t>Carma</t>
+  </si>
+  <si>
+    <t>Criminoso</t>
+  </si>
+  <si>
+    <t>Enfraquecimento e Recuperação</t>
+  </si>
+  <si>
+    <t>Deterioração dos Equipamentos por Ácido</t>
+  </si>
+  <si>
+    <t>Fé e Orações</t>
+  </si>
+  <si>
+    <t>Morte e Consequências</t>
+  </si>
+  <si>
+    <t>Ressurreição de Companheiros e Moradores</t>
+  </si>
+  <si>
+    <t>Fim da Infância</t>
+  </si>
+  <si>
+    <t>Água Perigosa</t>
+  </si>
+  <si>
+    <t>Doença do Éter</t>
+  </si>
+  <si>
+    <t>Ponto de Parada do Mercador Viajante</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Grau de Influência</t>
+  </si>
+  <si>
+    <t>Caixa de Entregas</t>
+  </si>
+  <si>
+    <t>Pedra da Cidade</t>
+  </si>
+  <si>
+    <t>Trabalhos e Hobbies dos Moradores</t>
+  </si>
+  <si>
+    <t>Pasto e Gado</t>
+  </si>
+  <si>
+    <t>Problema com o Lixo</t>
+  </si>
+  <si>
+    <t>Estações do Ano</t>
+  </si>
+  <si>
+    <t>Nerun Demo</t>
   </si>
 </sst>
 </file>
@@ -3264,8 +3264,8 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -3323,7 +3323,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>627</v>
+        <v>711</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3346,7 +3346,7 @@
         <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>628</v>
+        <v>712</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3369,7 +3369,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>629</v>
+        <v>713</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3392,7 +3392,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>630</v>
+        <v>714</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3415,7 +3415,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>631</v>
+        <v>715</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3438,7 +3438,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>632</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3461,7 +3461,7 @@
         <v>29</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>622</v>
+        <v>717</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3484,7 +3484,7 @@
         <v>32</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>615</v>
+        <v>718</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3507,7 +3507,7 @@
         <v>35</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>633</v>
+        <v>719</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3530,7 +3530,7 @@
         <v>38</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>616</v>
+        <v>720</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3553,7 +3553,7 @@
         <v>41</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>634</v>
+        <v>721</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3576,7 +3576,7 @@
         <v>44</v>
       </c>
       <c r="H16" t="s">
-        <v>617</v>
+        <v>722</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3599,7 +3599,7 @@
         <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>635</v>
+        <v>723</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -3622,7 +3622,7 @@
         <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>618</v>
+        <v>724</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3645,7 +3645,7 @@
         <v>53</v>
       </c>
       <c r="H19" t="s">
-        <v>636</v>
+        <v>725</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3668,7 +3668,7 @@
         <v>56</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>637</v>
+        <v>726</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3691,7 +3691,7 @@
         <v>59</v>
       </c>
       <c r="H21" t="s">
-        <v>623</v>
+        <v>727</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3714,7 +3714,7 @@
         <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>638</v>
+        <v>728</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3737,7 +3737,7 @@
         <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>639</v>
+        <v>729</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3760,7 +3760,7 @@
         <v>68</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>619</v>
+        <v>730</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3783,7 +3783,7 @@
         <v>71</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>620</v>
+        <v>731</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -3806,7 +3806,7 @@
         <v>74</v>
       </c>
       <c r="H26" t="s">
-        <v>624</v>
+        <v>732</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -3829,7 +3829,7 @@
         <v>77</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>640</v>
+        <v>733</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3853,7 +3853,7 @@
         <v>80</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>641</v>
+        <v>734</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -3877,7 +3877,7 @@
         <v>83</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>642</v>
+        <v>735</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -3901,7 +3901,7 @@
         <v>86</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>625</v>
+        <v>736</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3925,7 +3925,7 @@
         <v>89</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -3949,7 +3949,7 @@
         <v>92</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>644</v>
+        <v>738</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -3973,7 +3973,7 @@
         <v>95</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>621</v>
+        <v>739</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -3997,7 +3997,7 @@
         <v>98</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>626</v>
+        <v>740</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -4021,7 +4021,7 @@
         <v>101</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>645</v>
+        <v>741</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -4044,7 +4044,7 @@
         <v>103</v>
       </c>
       <c r="H36" t="s">
-        <v>646</v>
+        <v>742</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -4067,7 +4067,7 @@
         <v>106</v>
       </c>
       <c r="H37" t="s">
-        <v>647</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -5783,7 +5783,7 @@
         <v>251</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>648</v>
+        <v>616</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -5877,7 +5877,7 @@
         <v>255</v>
       </c>
       <c r="K137" s="3" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="33">
@@ -5898,7 +5898,7 @@
         <v>257</v>
       </c>
       <c r="K138" s="3" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
     </row>
     <row r="139" spans="1:11" ht="33">
@@ -5919,7 +5919,7 @@
         <v>259</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
     </row>
     <row r="140" spans="1:11" ht="66">
@@ -5961,7 +5961,7 @@
         <v>263</v>
       </c>
       <c r="K141" s="3" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
     </row>
     <row r="142" spans="1:11" ht="49.5">
@@ -5982,7 +5982,7 @@
         <v>265</v>
       </c>
       <c r="K142" s="3" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
     </row>
     <row r="143" spans="1:11" ht="33">
@@ -6064,7 +6064,7 @@
         <v>269</v>
       </c>
       <c r="K147" s="9" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -6082,7 +6082,7 @@
         <v>270</v>
       </c>
       <c r="J148" t="s">
-        <v>655</v>
+        <v>623</v>
       </c>
       <c r="K148" s="9" t="s">
         <v>519</v>
@@ -6106,7 +6106,7 @@
         <v>272</v>
       </c>
       <c r="K149" s="9" t="s">
-        <v>656</v>
+        <v>624</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="43.5">
@@ -6124,7 +6124,7 @@
         <v>273</v>
       </c>
       <c r="J150" s="9" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
       <c r="K150" s="9" t="s">
         <v>520</v>
@@ -6281,7 +6281,7 @@
         <v>285</v>
       </c>
       <c r="K158" s="3" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
     </row>
     <row r="159" spans="1:11" ht="99">
@@ -6375,7 +6375,7 @@
         <v>289</v>
       </c>
       <c r="K164" s="9" t="s">
-        <v>659</v>
+        <v>627</v>
       </c>
     </row>
     <row r="165" spans="1:11">
@@ -6396,7 +6396,7 @@
         <v>291</v>
       </c>
       <c r="K165" t="s">
-        <v>660</v>
+        <v>628</v>
       </c>
     </row>
     <row r="166" spans="1:11" ht="66">
@@ -6417,7 +6417,7 @@
         <v>293</v>
       </c>
       <c r="K166" s="3" t="s">
-        <v>664</v>
+        <v>632</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="66">
@@ -6438,7 +6438,7 @@
         <v>295</v>
       </c>
       <c r="K167" s="3" t="s">
-        <v>663</v>
+        <v>631</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="66">
@@ -6459,7 +6459,7 @@
         <v>297</v>
       </c>
       <c r="K168" s="3" t="s">
-        <v>661</v>
+        <v>629</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="49.5">
@@ -6480,7 +6480,7 @@
         <v>299</v>
       </c>
       <c r="K169" s="3" t="s">
-        <v>662</v>
+        <v>630</v>
       </c>
     </row>
     <row r="170" spans="1:11" ht="49.5">
@@ -6501,7 +6501,7 @@
         <v>301</v>
       </c>
       <c r="K170" s="3" t="s">
-        <v>665</v>
+        <v>633</v>
       </c>
     </row>
     <row r="171" spans="1:11">
@@ -6551,7 +6551,7 @@
         <v>305</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>666</v>
+        <v>634</v>
       </c>
     </row>
     <row r="177" spans="1:11" ht="49.5">
@@ -6565,7 +6565,7 @@
         <v>307</v>
       </c>
       <c r="K177" s="3" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
     </row>
     <row r="178" spans="1:11" ht="49.5">
@@ -6579,7 +6579,7 @@
         <v>309</v>
       </c>
       <c r="K178" s="3" t="s">
-        <v>668</v>
+        <v>636</v>
       </c>
     </row>
     <row r="179" spans="1:11" ht="33">
@@ -6593,7 +6593,7 @@
         <v>311</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>669</v>
+        <v>637</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -6617,7 +6617,7 @@
         <v>313</v>
       </c>
       <c r="K183" t="s">
-        <v>670</v>
+        <v>638</v>
       </c>
     </row>
     <row r="184" spans="1:11" ht="33">
@@ -6631,7 +6631,7 @@
         <v>315</v>
       </c>
       <c r="K184" s="9" t="s">
-        <v>671</v>
+        <v>639</v>
       </c>
     </row>
     <row r="185" spans="1:11" ht="33">
@@ -6645,7 +6645,7 @@
         <v>317</v>
       </c>
       <c r="K185" s="9" t="s">
-        <v>672</v>
+        <v>640</v>
       </c>
     </row>
     <row r="186" spans="1:11" ht="66">
@@ -6659,7 +6659,7 @@
         <v>319</v>
       </c>
       <c r="K186" s="9" t="s">
-        <v>673</v>
+        <v>641</v>
       </c>
     </row>
     <row r="187" spans="1:11" ht="40.5">
@@ -6673,7 +6673,7 @@
         <v>321</v>
       </c>
       <c r="K187" s="9" t="s">
-        <v>674</v>
+        <v>642</v>
       </c>
     </row>
     <row r="188" spans="1:11" ht="40.5">
@@ -6687,7 +6687,7 @@
         <v>323</v>
       </c>
       <c r="K188" s="9" t="s">
-        <v>675</v>
+        <v>643</v>
       </c>
     </row>
     <row r="189" spans="1:11">
@@ -6728,7 +6728,7 @@
         <v>327</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>676</v>
+        <v>644</v>
       </c>
     </row>
     <row r="195" spans="1:11" ht="33">
@@ -6742,7 +6742,7 @@
         <v>329</v>
       </c>
       <c r="K195" s="3" t="s">
-        <v>677</v>
+        <v>645</v>
       </c>
     </row>
     <row r="196" spans="1:11" ht="115.5">
@@ -6756,7 +6756,7 @@
         <v>331</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>678</v>
+        <v>646</v>
       </c>
     </row>
     <row r="197" spans="1:11" ht="82.5">
@@ -6770,7 +6770,7 @@
         <v>333</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>679</v>
+        <v>647</v>
       </c>
     </row>
     <row r="198" spans="1:11" ht="33">
@@ -6784,7 +6784,7 @@
         <v>335</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>680</v>
+        <v>648</v>
       </c>
     </row>
     <row r="199" spans="1:11">
@@ -6812,7 +6812,7 @@
         <v>337</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>681</v>
+        <v>649</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -6826,7 +6826,7 @@
         <v>339</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>682</v>
+        <v>650</v>
       </c>
     </row>
     <row r="202" spans="1:11">
@@ -6853,7 +6853,7 @@
         <v>341</v>
       </c>
       <c r="K208" t="s">
-        <v>683</v>
+        <v>651</v>
       </c>
     </row>
     <row r="209" spans="1:11">
@@ -6920,7 +6920,7 @@
         <v>350</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>684</v>
+        <v>652</v>
       </c>
     </row>
     <row r="214" spans="1:11" ht="66">
@@ -6934,7 +6934,7 @@
         <v>352</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
     </row>
     <row r="215" spans="1:11" ht="49.5">
@@ -6948,7 +6948,7 @@
         <v>354</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>686</v>
+        <v>654</v>
       </c>
     </row>
     <row r="216" spans="1:11" ht="33">
@@ -6962,7 +6962,7 @@
         <v>356</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>687</v>
+        <v>655</v>
       </c>
     </row>
     <row r="217" spans="1:11" ht="33">
@@ -6976,7 +6976,7 @@
         <v>358</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
     </row>
     <row r="218" spans="1:11" ht="82.5">
@@ -6990,7 +6990,7 @@
         <v>360</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
     </row>
     <row r="219" spans="1:11">
@@ -7018,7 +7018,7 @@
         <v>362</v>
       </c>
       <c r="K221" s="9" t="s">
-        <v>690</v>
+        <v>658</v>
       </c>
     </row>
     <row r="222" spans="1:11">
@@ -7084,7 +7084,7 @@
         <v>370</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>691</v>
+        <v>659</v>
       </c>
     </row>
     <row r="229" spans="1:11">
@@ -7109,7 +7109,7 @@
         <v>371</v>
       </c>
       <c r="J230" s="3" t="s">
-        <v>692</v>
+        <v>660</v>
       </c>
       <c r="K230" s="3" t="s">
         <v>534</v>
@@ -7126,7 +7126,7 @@
         <v>373</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>693</v>
+        <v>661</v>
       </c>
     </row>
     <row r="232" spans="1:11">
@@ -7197,7 +7197,7 @@
         <v>381</v>
       </c>
       <c r="K238" s="3" t="s">
-        <v>694</v>
+        <v>662</v>
       </c>
     </row>
     <row r="239" spans="1:11">
@@ -7211,7 +7211,7 @@
         <v>383</v>
       </c>
       <c r="K239" t="s">
-        <v>695</v>
+        <v>663</v>
       </c>
     </row>
     <row r="240" spans="1:11">
@@ -7257,7 +7257,7 @@
         <v>385</v>
       </c>
       <c r="K245" t="s">
-        <v>696</v>
+        <v>664</v>
       </c>
     </row>
     <row r="246" spans="1:11" ht="66">
@@ -7271,7 +7271,7 @@
         <v>387</v>
       </c>
       <c r="K246" s="3" t="s">
-        <v>697</v>
+        <v>665</v>
       </c>
     </row>
     <row r="247" spans="1:11" ht="49.5">
@@ -7285,7 +7285,7 @@
         <v>389</v>
       </c>
       <c r="K247" s="3" t="s">
-        <v>698</v>
+        <v>666</v>
       </c>
     </row>
     <row r="248" spans="1:11" ht="82.5">
@@ -7299,7 +7299,7 @@
         <v>391</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>699</v>
+        <v>667</v>
       </c>
     </row>
     <row r="249" spans="1:11">
@@ -7313,7 +7313,7 @@
         <v>393</v>
       </c>
       <c r="K249" t="s">
-        <v>700</v>
+        <v>668</v>
       </c>
     </row>
     <row r="250" spans="1:11">
@@ -7373,7 +7373,7 @@
         <v>397</v>
       </c>
       <c r="K256" s="3" t="s">
-        <v>701</v>
+        <v>669</v>
       </c>
     </row>
     <row r="257" spans="1:11" ht="115.5">
@@ -7381,13 +7381,13 @@
         <v>88</v>
       </c>
       <c r="I257" s="3" t="s">
-        <v>703</v>
+        <v>671</v>
       </c>
       <c r="J257" s="3" t="s">
         <v>398</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>702</v>
+        <v>670</v>
       </c>
     </row>
     <row r="258" spans="1:11" ht="99">
@@ -7401,7 +7401,7 @@
         <v>400</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>704</v>
+        <v>672</v>
       </c>
     </row>
     <row r="259" spans="1:11" ht="49.5">
@@ -7429,7 +7429,7 @@
         <v>404</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>705</v>
+        <v>673</v>
       </c>
     </row>
     <row r="261" spans="1:11">
@@ -7443,7 +7443,7 @@
         <v>405</v>
       </c>
       <c r="K261" t="s">
-        <v>706</v>
+        <v>674</v>
       </c>
     </row>
     <row r="262" spans="1:11">
@@ -7467,7 +7467,7 @@
         <v>407</v>
       </c>
       <c r="K265" t="s">
-        <v>707</v>
+        <v>675</v>
       </c>
     </row>
     <row r="266" spans="1:11" ht="49.5">
@@ -7481,7 +7481,7 @@
         <v>409</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>708</v>
+        <v>676</v>
       </c>
     </row>
     <row r="267" spans="1:11" ht="99">
@@ -7495,7 +7495,7 @@
         <v>411</v>
       </c>
       <c r="K267" s="3" t="s">
-        <v>709</v>
+        <v>677</v>
       </c>
     </row>
     <row r="268" spans="1:11" ht="33">
@@ -7509,7 +7509,7 @@
         <v>413</v>
       </c>
       <c r="K268" s="3" t="s">
-        <v>710</v>
+        <v>678</v>
       </c>
     </row>
     <row r="269" spans="1:11" ht="82.5">
@@ -7523,7 +7523,7 @@
         <v>415</v>
       </c>
       <c r="K269" s="3" t="s">
-        <v>711</v>
+        <v>679</v>
       </c>
     </row>
     <row r="270" spans="1:11">
@@ -7557,7 +7557,7 @@
         <v>417</v>
       </c>
       <c r="K275" s="9" t="s">
-        <v>712</v>
+        <v>680</v>
       </c>
     </row>
     <row r="276" spans="1:11" ht="33">
@@ -7571,7 +7571,7 @@
         <v>419</v>
       </c>
       <c r="K276" s="3" t="s">
-        <v>713</v>
+        <v>681</v>
       </c>
     </row>
     <row r="277" spans="1:11">
@@ -7582,7 +7582,7 @@
         <v>420</v>
       </c>
       <c r="J277" s="3" t="s">
-        <v>714</v>
+        <v>682</v>
       </c>
       <c r="K277" s="3" t="s">
         <v>540</v>
@@ -7613,7 +7613,7 @@
         <v>424</v>
       </c>
       <c r="K279" s="3" t="s">
-        <v>715</v>
+        <v>683</v>
       </c>
     </row>
     <row r="280" spans="1:11" ht="66">
@@ -7627,7 +7627,7 @@
         <v>426</v>
       </c>
       <c r="K280" s="3" t="s">
-        <v>716</v>
+        <v>684</v>
       </c>
     </row>
     <row r="281" spans="1:11" ht="49.5">
@@ -7641,7 +7641,7 @@
         <v>428</v>
       </c>
       <c r="K281" s="3" t="s">
-        <v>717</v>
+        <v>685</v>
       </c>
     </row>
     <row r="282" spans="1:11" ht="33">
@@ -7655,7 +7655,7 @@
         <v>430</v>
       </c>
       <c r="K282" s="3" t="s">
-        <v>718</v>
+        <v>686</v>
       </c>
     </row>
     <row r="283" spans="1:11">
@@ -7679,7 +7679,7 @@
         <v>432</v>
       </c>
       <c r="K285" t="s">
-        <v>719</v>
+        <v>687</v>
       </c>
     </row>
     <row r="286" spans="1:11" ht="99">
@@ -7707,7 +7707,7 @@
         <v>436</v>
       </c>
       <c r="K287" s="3" t="s">
-        <v>720</v>
+        <v>688</v>
       </c>
     </row>
     <row r="288" spans="1:11" ht="66">
@@ -7721,7 +7721,7 @@
         <v>438</v>
       </c>
       <c r="K288" s="3" t="s">
-        <v>721</v>
+        <v>689</v>
       </c>
     </row>
     <row r="289" spans="1:11" ht="49.5">
@@ -7735,7 +7735,7 @@
         <v>440</v>
       </c>
       <c r="K289" s="3" t="s">
-        <v>722</v>
+        <v>690</v>
       </c>
     </row>
     <row r="290" spans="1:11" ht="49.5">
@@ -7749,7 +7749,7 @@
         <v>442</v>
       </c>
       <c r="K290" s="3" t="s">
-        <v>723</v>
+        <v>691</v>
       </c>
     </row>
     <row r="291" spans="1:11">
@@ -7801,7 +7801,7 @@
         <v>448</v>
       </c>
       <c r="K297" s="9" t="s">
-        <v>724</v>
+        <v>692</v>
       </c>
     </row>
     <row r="298" spans="1:11" ht="33">
@@ -7815,7 +7815,7 @@
         <v>450</v>
       </c>
       <c r="K298" s="9" t="s">
-        <v>725</v>
+        <v>693</v>
       </c>
     </row>
     <row r="299" spans="1:11">
@@ -7857,7 +7857,7 @@
         <v>166</v>
       </c>
       <c r="K301" s="9" t="s">
-        <v>726</v>
+        <v>694</v>
       </c>
     </row>
     <row r="302" spans="1:11">
@@ -7881,7 +7881,7 @@
         <v>454</v>
       </c>
       <c r="K307" t="s">
-        <v>727</v>
+        <v>695</v>
       </c>
     </row>
     <row r="308" spans="1:11" ht="33">
@@ -7895,7 +7895,7 @@
         <v>456</v>
       </c>
       <c r="K308" s="3" t="s">
-        <v>728</v>
+        <v>696</v>
       </c>
     </row>
     <row r="309" spans="1:11" ht="49.5">
@@ -7909,7 +7909,7 @@
         <v>458</v>
       </c>
       <c r="K309" s="3" t="s">
-        <v>729</v>
+        <v>697</v>
       </c>
     </row>
     <row r="310" spans="1:11" ht="49.5">
@@ -7923,7 +7923,7 @@
         <v>460</v>
       </c>
       <c r="K310" s="9" t="s">
-        <v>730</v>
+        <v>698</v>
       </c>
     </row>
     <row r="311" spans="1:11" ht="99">
@@ -7937,7 +7937,7 @@
         <v>462</v>
       </c>
       <c r="K311" s="3" t="s">
-        <v>731</v>
+        <v>699</v>
       </c>
     </row>
     <row r="312" spans="1:11" ht="33">
@@ -7951,7 +7951,7 @@
         <v>464</v>
       </c>
       <c r="K312" s="3" t="s">
-        <v>732</v>
+        <v>700</v>
       </c>
     </row>
     <row r="313" spans="1:11">
@@ -7975,7 +7975,7 @@
         <v>466</v>
       </c>
       <c r="K317" s="3" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
     </row>
     <row r="318" spans="1:11" ht="33">
@@ -7989,7 +7989,7 @@
         <v>468</v>
       </c>
       <c r="K318" s="3" t="s">
-        <v>734</v>
+        <v>702</v>
       </c>
     </row>
     <row r="319" spans="1:11" ht="49.5">
@@ -8003,7 +8003,7 @@
         <v>470</v>
       </c>
       <c r="K319" s="3" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
     </row>
     <row r="320" spans="1:11" ht="66">
@@ -8017,7 +8017,7 @@
         <v>472</v>
       </c>
       <c r="K320" s="3" t="s">
-        <v>736</v>
+        <v>704</v>
       </c>
     </row>
     <row r="321" spans="1:11" ht="99">
@@ -8031,7 +8031,7 @@
         <v>474</v>
       </c>
       <c r="K321" s="3" t="s">
-        <v>737</v>
+        <v>705</v>
       </c>
     </row>
     <row r="322" spans="1:11" ht="33">
@@ -8045,7 +8045,7 @@
         <v>476</v>
       </c>
       <c r="K322" s="3" t="s">
-        <v>738</v>
+        <v>706</v>
       </c>
     </row>
     <row r="323" spans="1:11" ht="115.5">
@@ -8059,7 +8059,7 @@
         <v>478</v>
       </c>
       <c r="K323" s="3" t="s">
-        <v>739</v>
+        <v>707</v>
       </c>
     </row>
     <row r="324" spans="1:11">
@@ -8073,7 +8073,7 @@
         <v>166</v>
       </c>
       <c r="K324" s="9" t="s">
-        <v>726</v>
+        <v>694</v>
       </c>
     </row>
     <row r="325" spans="1:11">
@@ -8119,7 +8119,7 @@
         <v>484</v>
       </c>
       <c r="K330" s="3" t="s">
-        <v>740</v>
+        <v>708</v>
       </c>
     </row>
     <row r="331" spans="1:11" ht="33">
@@ -8173,7 +8173,7 @@
         <v>492</v>
       </c>
       <c r="K335" t="s">
-        <v>741</v>
+        <v>709</v>
       </c>
     </row>
     <row r="336" spans="1:11">
@@ -8238,7 +8238,7 @@
         <v>500</v>
       </c>
       <c r="K342" t="s">
-        <v>742</v>
+        <v>710</v>
       </c>
     </row>
     <row r="343" spans="1:11">

</xml_diff>